<commit_message>
Still working on DataStructure Functionality
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Rajesh\Doxy_CycD1_CycE1_P27__Drug_Treatment_Exps\For Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Justin S\Experiments\Growth Rate\Cell Cycle Length Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="23550" windowHeight="11265"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="23550" windowHeight="11265"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="108">
   <si>
     <t>Path to Dataset</t>
   </si>
@@ -317,6 +317,33 @@
   </si>
   <si>
     <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171030_JS_cycD_26HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171030_JS_p27_42HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171030_JS_p27_47HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171030_JS_p27_66HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171030_JS_cycE_42HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171030_JS_cycE_47HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171030_JS_cycE_66HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171030_JS_cycD_42HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171030_JS_cycD_47HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171030_JS_cycD_66HrRESULTS</t>
   </si>
 </sst>
 </file>
@@ -633,8 +660,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K63" totalsRowShown="0">
-  <autoFilter ref="A1:K63"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K67" totalsRowShown="0">
+  <autoFilter ref="A1:K67"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Path to Dataset" dataCellStyle="Hyperlink"/>
     <tableColumn id="2" name="Plate_Map" dataCellStyle="Hyperlink"/>
@@ -915,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M60" sqref="M60"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2555,7 +2582,9 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
+      <c r="A51" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="B51" s="1" t="s">
         <v>86</v>
       </c>
@@ -2585,7 +2614,9 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
+      <c r="A52" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="B52" s="1" t="s">
         <v>86</v>
       </c>
@@ -2601,6 +2632,9 @@
       <c r="F52" t="s">
         <v>87</v>
       </c>
+      <c r="G52">
+        <v>47</v>
+      </c>
       <c r="H52" t="s">
         <v>5</v>
       </c>
@@ -2613,7 +2647,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>86</v>
@@ -2622,22 +2656,22 @@
         <v>27</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>77</v>
       </c>
       <c r="F53" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="H53" t="s">
         <v>5</v>
       </c>
       <c r="I53" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="K53" s="2">
         <v>43038</v>
@@ -2645,7 +2679,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>86</v>
@@ -2663,7 +2697,7 @@
         <v>88</v>
       </c>
       <c r="G54">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H54" t="s">
         <v>5</v>
@@ -2677,7 +2711,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>86</v>
@@ -2695,7 +2729,7 @@
         <v>88</v>
       </c>
       <c r="G55">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H55" t="s">
         <v>5</v>
@@ -2709,7 +2743,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>86</v>
@@ -2727,7 +2761,7 @@
         <v>88</v>
       </c>
       <c r="G56">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H56" t="s">
         <v>5</v>
@@ -2740,7 +2774,9 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
+      <c r="A57" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="B57" s="1" t="s">
         <v>86</v>
       </c>
@@ -2757,7 +2793,7 @@
         <v>88</v>
       </c>
       <c r="G57">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="H57" t="s">
         <v>5</v>
@@ -2770,7 +2806,9 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
+      <c r="A58" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="B58" s="1" t="s">
         <v>86</v>
       </c>
@@ -2786,6 +2824,9 @@
       <c r="F58" t="s">
         <v>88</v>
       </c>
+      <c r="G58">
+        <v>42</v>
+      </c>
       <c r="H58" t="s">
         <v>5</v>
       </c>
@@ -2798,7 +2839,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>86</v>
@@ -2807,22 +2848,22 @@
         <v>27</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>77</v>
       </c>
       <c r="F59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G59">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="H59" t="s">
         <v>5</v>
       </c>
       <c r="I59" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K59" s="2">
         <v>43038</v>
@@ -2830,7 +2871,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>86</v>
@@ -2839,22 +2880,22 @@
         <v>27</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>77</v>
       </c>
       <c r="F60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G60">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="H60" t="s">
         <v>5</v>
       </c>
       <c r="I60" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K60" s="2">
         <v>43038</v>
@@ -2862,7 +2903,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>86</v>
@@ -2880,7 +2921,7 @@
         <v>89</v>
       </c>
       <c r="G61">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H61" t="s">
         <v>5</v>
@@ -2894,7 +2935,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>86</v>
@@ -2912,7 +2953,7 @@
         <v>89</v>
       </c>
       <c r="G62">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="H62" t="s">
         <v>5</v>
@@ -2925,7 +2966,9 @@
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
+      <c r="A63" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="B63" s="1" t="s">
         <v>86</v>
       </c>
@@ -2942,7 +2985,7 @@
         <v>89</v>
       </c>
       <c r="G63">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="H63" t="s">
         <v>5</v>
@@ -2951,6 +2994,134 @@
         <v>78</v>
       </c>
       <c r="K63" s="2">
+        <v>43038</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F64" t="s">
+        <v>89</v>
+      </c>
+      <c r="G64">
+        <v>26</v>
+      </c>
+      <c r="H64" t="s">
+        <v>5</v>
+      </c>
+      <c r="I64" t="s">
+        <v>78</v>
+      </c>
+      <c r="K64" s="2">
+        <v>43038</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F65" t="s">
+        <v>89</v>
+      </c>
+      <c r="G65">
+        <v>42</v>
+      </c>
+      <c r="H65" t="s">
+        <v>5</v>
+      </c>
+      <c r="I65" t="s">
+        <v>78</v>
+      </c>
+      <c r="K65" s="2">
+        <v>43038</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F66" t="s">
+        <v>89</v>
+      </c>
+      <c r="G66">
+        <v>47</v>
+      </c>
+      <c r="H66" t="s">
+        <v>5</v>
+      </c>
+      <c r="I66" t="s">
+        <v>78</v>
+      </c>
+      <c r="K66" s="2">
+        <v>43038</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F67" t="s">
+        <v>89</v>
+      </c>
+      <c r="G67">
+        <v>66</v>
+      </c>
+      <c r="H67" t="s">
+        <v>5</v>
+      </c>
+      <c r="I67" t="s">
+        <v>78</v>
+      </c>
+      <c r="K67" s="2">
         <v>43038</v>
       </c>
     </row>
@@ -2970,17 +3141,15 @@
     <hyperlink ref="A46" r:id="rId12"/>
     <hyperlink ref="B26" r:id="rId13"/>
     <hyperlink ref="B27:B46" r:id="rId14" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171024_D1_E1_P27.xlsx"/>
-    <hyperlink ref="A53" r:id="rId15"/>
+    <hyperlink ref="A54" r:id="rId15"/>
     <hyperlink ref="B47" r:id="rId16"/>
-    <hyperlink ref="B48:B60" r:id="rId17" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171030_D1_E1_P27.xlsx"/>
-    <hyperlink ref="A47" r:id="rId18"/>
-    <hyperlink ref="A59" r:id="rId19"/>
-    <hyperlink ref="B49:B63" r:id="rId20" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171030_D1_E1_P27.xlsx"/>
+    <hyperlink ref="A47" r:id="rId17"/>
+    <hyperlink ref="A61" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
   <tableParts count="1">
-    <tablePart r:id="rId22"/>
+    <tablePart r:id="rId20"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Separated DPC analysis into a separate function, and added an SE analysis function.
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="23550" windowHeight="11265"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="23550" windowHeight="11265"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="116">
   <si>
     <t>Path to Dataset</t>
   </si>
@@ -31,30 +31,12 @@
     <t>Cell Line</t>
   </si>
   <si>
-    <t>Colour</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
     <t>RPE1</t>
   </si>
   <si>
-    <t>[.5 .5 .5]</t>
-  </si>
-  <si>
-    <t>[1 .4 .4]</t>
-  </si>
-  <si>
-    <t>[.3 .8 .3]</t>
-  </si>
-  <si>
-    <t>[.4 .4 1]</t>
-  </si>
-  <si>
-    <t>[0.6 0.2 0.4]</t>
-  </si>
-  <si>
     <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20170926_cycD1RESULTS</t>
   </si>
   <si>
@@ -344,6 +326,48 @@
   </si>
   <si>
     <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171030_JS_cycD_66HrRESULTS</t>
+  </si>
+  <si>
+    <t>Imaging_Type</t>
+  </si>
+  <si>
+    <t>DPC</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20170926_cycD1_RGRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20170926_cycE1_RG_repeatRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171003_cycD1_DAPI_alexa_647RESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171003_cycE1_DAPE_Alexa647RESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171003_P27__DAPI_Alexa_647RESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171024_JS_CycD1_SERESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171024_JS_CycE1_SERESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171024_JS_p27_SERESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171030_JS_cycD_SERESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171030_JS_cycE_SERESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171030_JS_p27_SERESULTS</t>
+  </si>
+  <si>
+    <t>SE</t>
   </si>
 </sst>
 </file>
@@ -660,8 +684,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K67" totalsRowShown="0">
-  <autoFilter ref="A1:K67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K78" totalsRowShown="0">
+  <autoFilter ref="A1:K78"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Path to Dataset" dataCellStyle="Hyperlink"/>
     <tableColumn id="2" name="Plate_Map" dataCellStyle="Hyperlink"/>
@@ -672,7 +696,7 @@
     <tableColumn id="6" name="Time-Point"/>
     <tableColumn id="10" name="Cell Line"/>
     <tableColumn id="7" name="Expression"/>
-    <tableColumn id="8" name="Colour"/>
+    <tableColumn id="8" name="Imaging_Type"/>
     <tableColumn id="9" name="Date" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -942,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,11 +979,11 @@
     <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.140625" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -968,19 +992,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
@@ -989,45 +1013,45 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
-      </c>
-      <c r="K1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J2" t="s">
-        <v>6</v>
+        <v>103</v>
       </c>
       <c r="K2" s="2">
         <v>43004</v>
@@ -1035,34 +1059,34 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G3">
         <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J3" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="K3" s="2">
         <v>43004</v>
@@ -1070,31 +1094,34 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>72</v>
+      </c>
+      <c r="J4" t="s">
+        <v>103</v>
       </c>
       <c r="K4" s="2">
         <v>43004</v>
@@ -1102,34 +1129,34 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G5">
         <v>42</v>
       </c>
       <c r="H5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J5" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="K5" s="2">
         <v>43004</v>
@@ -1137,34 +1164,34 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G6">
         <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J6" t="s">
-        <v>9</v>
+        <v>103</v>
       </c>
       <c r="K6" s="2">
         <v>43004</v>
@@ -1172,34 +1199,34 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G7">
         <v>67</v>
       </c>
       <c r="H7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J7" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="K7" s="2">
         <v>43004</v>
@@ -1207,31 +1234,34 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>104</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="H8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>79</v>
+        <v>72</v>
+      </c>
+      <c r="J8" t="s">
+        <v>115</v>
       </c>
       <c r="K8" s="2">
         <v>43004</v>
@@ -1239,31 +1269,34 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G9">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I9" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="J9" t="s">
+        <v>103</v>
       </c>
       <c r="K9" s="2">
         <v>43004</v>
@@ -1271,31 +1304,34 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10">
         <v>18</v>
       </c>
-      <c r="G10">
-        <v>24</v>
-      </c>
       <c r="H10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I10" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="J10" t="s">
+        <v>103</v>
       </c>
       <c r="K10" s="2">
         <v>43004</v>
@@ -1303,31 +1339,34 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G11">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="H11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I11" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="J11" t="s">
+        <v>103</v>
       </c>
       <c r="K11" s="2">
         <v>43004</v>
@@ -1335,31 +1374,34 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G12">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I12" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="J12" t="s">
+        <v>103</v>
       </c>
       <c r="K12" s="2">
         <v>43004</v>
@@ -1367,31 +1409,34 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G13">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="H13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I13" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="J13" t="s">
+        <v>103</v>
       </c>
       <c r="K13" s="2">
         <v>43004</v>
@@ -1399,95 +1444,104 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="H14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>78</v>
+        <v>73</v>
+      </c>
+      <c r="J14" t="s">
+        <v>103</v>
       </c>
       <c r="K14" s="2">
-        <v>43011</v>
+        <v>43004</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="G15">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="H15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I15" t="s">
-        <v>78</v>
+        <v>73</v>
+      </c>
+      <c r="J15" t="s">
+        <v>115</v>
       </c>
       <c r="K15" s="2">
-        <v>43011</v>
+        <v>43004</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G16">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I16" t="s">
-        <v>78</v>
+        <v>72</v>
+      </c>
+      <c r="J16" t="s">
+        <v>103</v>
       </c>
       <c r="K16" s="2">
         <v>43011</v>
@@ -1495,31 +1549,34 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F17" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G17">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="H17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I17" t="s">
-        <v>78</v>
+        <v>72</v>
+      </c>
+      <c r="J17" t="s">
+        <v>103</v>
       </c>
       <c r="K17" s="2">
         <v>43011</v>
@@ -1527,31 +1584,34 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="G18">
         <v>44</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
       <c r="H18" t="s">
-        <v>5</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>79</v>
+        <v>4</v>
+      </c>
+      <c r="I18" t="s">
+        <v>72</v>
+      </c>
+      <c r="J18" t="s">
+        <v>103</v>
       </c>
       <c r="K18" s="2">
         <v>43011</v>
@@ -1559,31 +1619,34 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F19" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G19">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="H19" t="s">
-        <v>5</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>79</v>
+        <v>4</v>
+      </c>
+      <c r="I19" t="s">
+        <v>72</v>
+      </c>
+      <c r="J19" t="s">
+        <v>103</v>
       </c>
       <c r="K19" s="2">
         <v>43011</v>
@@ -1591,31 +1654,34 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F20" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G20">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="H20" t="s">
-        <v>5</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>79</v>
+        <v>4</v>
+      </c>
+      <c r="I20" t="s">
+        <v>72</v>
+      </c>
+      <c r="J20" t="s">
+        <v>115</v>
       </c>
       <c r="K20" s="2">
         <v>43011</v>
@@ -1623,31 +1689,34 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F21" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G21">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="J21" t="s">
+        <v>103</v>
       </c>
       <c r="K21" s="2">
         <v>43011</v>
@@ -1655,31 +1724,34 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F22" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H22" t="s">
-        <v>5</v>
-      </c>
-      <c r="I22" t="s">
-        <v>46</v>
+        <v>4</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J22" t="s">
+        <v>103</v>
       </c>
       <c r="K22" s="2">
         <v>43011</v>
@@ -1687,31 +1759,34 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23">
         <v>44</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23">
-        <v>20</v>
-      </c>
       <c r="H23" t="s">
-        <v>5</v>
-      </c>
-      <c r="I23" t="s">
-        <v>46</v>
+        <v>4</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J23" t="s">
+        <v>103</v>
       </c>
       <c r="K23" s="2">
         <v>43011</v>
@@ -1719,31 +1794,34 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C24" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F24" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G24">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="H24" t="s">
-        <v>5</v>
-      </c>
-      <c r="I24" t="s">
-        <v>46</v>
+        <v>4</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J24" t="s">
+        <v>103</v>
       </c>
       <c r="K24" s="2">
         <v>43011</v>
@@ -1751,31 +1829,34 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F25" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G25">
         <v>65</v>
       </c>
       <c r="H25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I25" t="s">
-        <v>46</v>
+        <v>73</v>
+      </c>
+      <c r="J25" t="s">
+        <v>115</v>
       </c>
       <c r="K25" s="2">
         <v>43011</v>
@@ -1783,191 +1864,209 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F26" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I26" t="s">
-        <v>78</v>
+        <v>40</v>
+      </c>
+      <c r="J26" t="s">
+        <v>103</v>
       </c>
       <c r="K26" s="2">
-        <v>43032</v>
+        <v>43011</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F27" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="G27">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I27" t="s">
-        <v>78</v>
+        <v>40</v>
+      </c>
+      <c r="J27" t="s">
+        <v>103</v>
       </c>
       <c r="K27" s="2">
-        <v>43032</v>
+        <v>43011</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F28" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="G28">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="H28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I28" t="s">
-        <v>78</v>
+        <v>40</v>
+      </c>
+      <c r="J28" t="s">
+        <v>103</v>
       </c>
       <c r="K28" s="2">
-        <v>43032</v>
+        <v>43011</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F29" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="G29">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="H29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I29" t="s">
-        <v>78</v>
+        <v>40</v>
+      </c>
+      <c r="J29" t="s">
+        <v>103</v>
       </c>
       <c r="K29" s="2">
-        <v>43032</v>
+        <v>43011</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F30" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="G30">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="H30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I30" t="s">
-        <v>78</v>
+        <v>40</v>
+      </c>
+      <c r="J30" t="s">
+        <v>115</v>
       </c>
       <c r="K30" s="2">
-        <v>43032</v>
+        <v>43011</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F31" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" t="s">
         <v>72</v>
       </c>
-      <c r="G31">
-        <v>63</v>
-      </c>
-      <c r="H31" t="s">
-        <v>5</v>
-      </c>
-      <c r="I31" t="s">
-        <v>78</v>
+      <c r="J31" t="s">
+        <v>103</v>
       </c>
       <c r="K31" s="2">
         <v>43032</v>
@@ -1975,31 +2074,34 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F32" t="s">
+        <v>66</v>
+      </c>
+      <c r="G32">
+        <v>18</v>
+      </c>
+      <c r="H32" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" t="s">
         <v>72</v>
       </c>
-      <c r="G32">
-        <v>69</v>
-      </c>
-      <c r="H32" t="s">
-        <v>5</v>
-      </c>
-      <c r="I32" t="s">
-        <v>78</v>
+      <c r="J32" t="s">
+        <v>103</v>
       </c>
       <c r="K32" s="2">
         <v>43032</v>
@@ -2007,31 +2109,34 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F33" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H33" t="s">
-        <v>5</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>79</v>
+        <v>4</v>
+      </c>
+      <c r="I33" t="s">
+        <v>72</v>
+      </c>
+      <c r="J33" t="s">
+        <v>103</v>
       </c>
       <c r="K33" s="2">
         <v>43032</v>
@@ -2039,31 +2144,34 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F34" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G34">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="H34" t="s">
-        <v>5</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>79</v>
+        <v>4</v>
+      </c>
+      <c r="I34" t="s">
+        <v>72</v>
+      </c>
+      <c r="J34" t="s">
+        <v>103</v>
       </c>
       <c r="K34" s="2">
         <v>43032</v>
@@ -2071,31 +2179,34 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F35" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G35">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="H35" t="s">
-        <v>5</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>79</v>
+        <v>4</v>
+      </c>
+      <c r="I35" t="s">
+        <v>72</v>
+      </c>
+      <c r="J35" t="s">
+        <v>103</v>
       </c>
       <c r="K35" s="2">
         <v>43032</v>
@@ -2103,31 +2214,34 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F36" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G36">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="H36" t="s">
-        <v>5</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>79</v>
+        <v>4</v>
+      </c>
+      <c r="I36" t="s">
+        <v>72</v>
+      </c>
+      <c r="J36" t="s">
+        <v>103</v>
       </c>
       <c r="K36" s="2">
         <v>43032</v>
@@ -2135,31 +2249,34 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F37" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G37">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="H37" t="s">
-        <v>5</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>79</v>
+        <v>4</v>
+      </c>
+      <c r="I37" t="s">
+        <v>72</v>
+      </c>
+      <c r="J37" t="s">
+        <v>103</v>
       </c>
       <c r="K37" s="2">
         <v>43032</v>
@@ -2167,31 +2284,34 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F38" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G38">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="H38" t="s">
-        <v>5</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>79</v>
+        <v>4</v>
+      </c>
+      <c r="I38" t="s">
+        <v>72</v>
+      </c>
+      <c r="J38" t="s">
+        <v>115</v>
       </c>
       <c r="K38" s="2">
         <v>43032</v>
@@ -2199,31 +2319,34 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F39" t="s">
+        <v>67</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39" t="s">
+        <v>4</v>
+      </c>
+      <c r="I39" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G39">
-        <v>69</v>
-      </c>
-      <c r="H39" t="s">
-        <v>5</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>79</v>
+      <c r="J39" t="s">
+        <v>103</v>
       </c>
       <c r="K39" s="2">
         <v>43032</v>
@@ -2231,31 +2354,34 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F40" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H40" t="s">
-        <v>5</v>
-      </c>
-      <c r="I40" t="s">
-        <v>46</v>
+        <v>4</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J40" t="s">
+        <v>103</v>
       </c>
       <c r="K40" s="2">
         <v>43032</v>
@@ -2263,31 +2389,34 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="C41" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F41" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G41">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H41" t="s">
-        <v>5</v>
-      </c>
-      <c r="I41" t="s">
-        <v>46</v>
+        <v>4</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J41" t="s">
+        <v>103</v>
       </c>
       <c r="K41" s="2">
         <v>43032</v>
@@ -2295,31 +2424,34 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F42" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G42">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H42" t="s">
-        <v>5</v>
-      </c>
-      <c r="I42" t="s">
-        <v>46</v>
+        <v>4</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J42" t="s">
+        <v>103</v>
       </c>
       <c r="K42" s="2">
         <v>43032</v>
@@ -2327,31 +2459,34 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F43" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G43">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H43" t="s">
-        <v>5</v>
-      </c>
-      <c r="I43" t="s">
-        <v>46</v>
+        <v>4</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J43" t="s">
+        <v>103</v>
       </c>
       <c r="K43" s="2">
         <v>43032</v>
@@ -2359,31 +2494,34 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F44" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F44" t="s">
-        <v>71</v>
-      </c>
       <c r="G44">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="H44" t="s">
-        <v>5</v>
-      </c>
-      <c r="I44" t="s">
-        <v>46</v>
+        <v>4</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J44" t="s">
+        <v>103</v>
       </c>
       <c r="K44" s="2">
         <v>43032</v>
@@ -2391,31 +2529,34 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="E45" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F45" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G45">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="H45" t="s">
-        <v>5</v>
-      </c>
-      <c r="I45" t="s">
-        <v>46</v>
+        <v>4</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J45" t="s">
+        <v>103</v>
       </c>
       <c r="K45" s="2">
         <v>43032</v>
@@ -2423,31 +2564,34 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F46" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G46">
         <v>69</v>
       </c>
       <c r="H46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I46" t="s">
-        <v>46</v>
+        <v>73</v>
+      </c>
+      <c r="J46" t="s">
+        <v>115</v>
       </c>
       <c r="K46" s="2">
         <v>43032</v>
@@ -2455,287 +2599,314 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F47" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="G47">
         <v>0</v>
       </c>
       <c r="H47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I47" t="s">
-        <v>46</v>
+        <v>40</v>
+      </c>
+      <c r="J47" t="s">
+        <v>103</v>
       </c>
       <c r="K47" s="2">
-        <v>43038</v>
+        <v>43032</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F48" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="G48">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I48" t="s">
-        <v>46</v>
+        <v>40</v>
+      </c>
+      <c r="J48" t="s">
+        <v>103</v>
       </c>
       <c r="K48" s="2">
-        <v>43038</v>
+        <v>43032</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F49" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="G49">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H49" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I49" t="s">
-        <v>46</v>
+        <v>40</v>
+      </c>
+      <c r="J49" t="s">
+        <v>103</v>
       </c>
       <c r="K49" s="2">
-        <v>43038</v>
+        <v>43032</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F50" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="G50">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="H50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I50" t="s">
-        <v>46</v>
+        <v>40</v>
+      </c>
+      <c r="J50" t="s">
+        <v>103</v>
       </c>
       <c r="K50" s="2">
-        <v>43038</v>
+        <v>43032</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F51" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="G51">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H51" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I51" t="s">
-        <v>46</v>
+        <v>40</v>
+      </c>
+      <c r="J51" t="s">
+        <v>103</v>
       </c>
       <c r="K51" s="2">
-        <v>43038</v>
+        <v>43032</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F52" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="G52">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="H52" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I52" t="s">
-        <v>46</v>
+        <v>40</v>
+      </c>
+      <c r="J52" t="s">
+        <v>103</v>
       </c>
       <c r="K52" s="2">
-        <v>43038</v>
+        <v>43032</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>101</v>
+        <v>63</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F53" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="G53">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I53" t="s">
-        <v>46</v>
+        <v>40</v>
+      </c>
+      <c r="J53" t="s">
+        <v>103</v>
       </c>
       <c r="K53" s="2">
-        <v>43038</v>
+        <v>43032</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F54" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="G54">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="H54" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I54" t="s">
-        <v>79</v>
+        <v>40</v>
+      </c>
+      <c r="J54" t="s">
+        <v>115</v>
       </c>
       <c r="K54" s="2">
-        <v>43038</v>
+        <v>43032</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F55" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G55">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I55" t="s">
-        <v>79</v>
+        <v>40</v>
+      </c>
+      <c r="J55" t="s">
+        <v>103</v>
       </c>
       <c r="K55" s="2">
         <v>43038</v>
@@ -2743,31 +2914,34 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F56" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G56">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H56" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I56" t="s">
-        <v>79</v>
+        <v>40</v>
+      </c>
+      <c r="J56" t="s">
+        <v>103</v>
       </c>
       <c r="K56" s="2">
         <v>43038</v>
@@ -2775,31 +2949,34 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F57" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G57">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I57" t="s">
-        <v>79</v>
+        <v>40</v>
+      </c>
+      <c r="J57" t="s">
+        <v>103</v>
       </c>
       <c r="K57" s="2">
         <v>43038</v>
@@ -2807,31 +2984,34 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F58" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G58">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="H58" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I58" t="s">
-        <v>79</v>
+        <v>40</v>
+      </c>
+      <c r="J58" t="s">
+        <v>103</v>
       </c>
       <c r="K58" s="2">
         <v>43038</v>
@@ -2839,31 +3019,34 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F59" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G59">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H59" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I59" t="s">
-        <v>79</v>
+        <v>40</v>
+      </c>
+      <c r="J59" t="s">
+        <v>103</v>
       </c>
       <c r="K59" s="2">
         <v>43038</v>
@@ -2871,31 +3054,34 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F60" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G60">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="H60" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I60" t="s">
-        <v>79</v>
+        <v>40</v>
+      </c>
+      <c r="J60" t="s">
+        <v>103</v>
       </c>
       <c r="K60" s="2">
         <v>43038</v>
@@ -2903,31 +3089,34 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F61" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="H61" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I61" t="s">
-        <v>78</v>
+        <v>40</v>
+      </c>
+      <c r="J61" t="s">
+        <v>103</v>
       </c>
       <c r="K61" s="2">
         <v>43038</v>
@@ -2935,31 +3124,34 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F62" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G62">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="H62" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I62" t="s">
-        <v>78</v>
+        <v>40</v>
+      </c>
+      <c r="J62" t="s">
+        <v>115</v>
       </c>
       <c r="K62" s="2">
         <v>43038</v>
@@ -2967,31 +3159,34 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F63" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G63">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H63" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I63" t="s">
-        <v>78</v>
+        <v>73</v>
+      </c>
+      <c r="J63" t="s">
+        <v>103</v>
       </c>
       <c r="K63" s="2">
         <v>43038</v>
@@ -2999,31 +3194,34 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F64" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G64">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="H64" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I64" t="s">
-        <v>78</v>
+        <v>73</v>
+      </c>
+      <c r="J64" t="s">
+        <v>103</v>
       </c>
       <c r="K64" s="2">
         <v>43038</v>
@@ -3031,31 +3229,34 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F65" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G65">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="H65" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I65" t="s">
-        <v>78</v>
+        <v>73</v>
+      </c>
+      <c r="J65" t="s">
+        <v>103</v>
       </c>
       <c r="K65" s="2">
         <v>43038</v>
@@ -3063,31 +3264,34 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F66" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G66">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="H66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I66" t="s">
-        <v>78</v>
+        <v>73</v>
+      </c>
+      <c r="J66" t="s">
+        <v>103</v>
       </c>
       <c r="K66" s="2">
         <v>43038</v>
@@ -3095,61 +3299,448 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F67" t="s">
+        <v>82</v>
+      </c>
+      <c r="G67">
+        <v>42</v>
+      </c>
+      <c r="H67" t="s">
+        <v>4</v>
+      </c>
+      <c r="I67" t="s">
+        <v>73</v>
+      </c>
+      <c r="J67" t="s">
+        <v>103</v>
+      </c>
+      <c r="K67" s="2">
+        <v>43038</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F68" t="s">
+        <v>82</v>
+      </c>
+      <c r="G68">
+        <v>47</v>
+      </c>
+      <c r="H68" t="s">
+        <v>4</v>
+      </c>
+      <c r="I68" t="s">
+        <v>73</v>
+      </c>
+      <c r="J68" t="s">
+        <v>103</v>
+      </c>
+      <c r="K68" s="2">
+        <v>43038</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F69" t="s">
+        <v>82</v>
+      </c>
+      <c r="G69">
+        <v>66</v>
+      </c>
+      <c r="H69" t="s">
+        <v>4</v>
+      </c>
+      <c r="I69" t="s">
+        <v>73</v>
+      </c>
+      <c r="J69" t="s">
+        <v>103</v>
+      </c>
+      <c r="K69" s="2">
+        <v>43038</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F70" t="s">
+        <v>82</v>
+      </c>
+      <c r="G70">
+        <v>66</v>
+      </c>
+      <c r="H70" t="s">
+        <v>4</v>
+      </c>
+      <c r="I70" t="s">
+        <v>73</v>
+      </c>
+      <c r="J70" t="s">
+        <v>115</v>
+      </c>
+      <c r="K70" s="2">
+        <v>43038</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F71" t="s">
+        <v>83</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71" t="s">
+        <v>4</v>
+      </c>
+      <c r="I71" t="s">
+        <v>72</v>
+      </c>
+      <c r="J71" t="s">
+        <v>103</v>
+      </c>
+      <c r="K71" s="2">
+        <v>43038</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F72" t="s">
+        <v>83</v>
+      </c>
+      <c r="G72">
+        <v>16</v>
+      </c>
+      <c r="H72" t="s">
+        <v>4</v>
+      </c>
+      <c r="I72" t="s">
+        <v>72</v>
+      </c>
+      <c r="J72" t="s">
+        <v>103</v>
+      </c>
+      <c r="K72" s="2">
+        <v>43038</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G67">
+      <c r="B73" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F73" t="s">
+        <v>83</v>
+      </c>
+      <c r="G73">
+        <v>21</v>
+      </c>
+      <c r="H73" t="s">
+        <v>4</v>
+      </c>
+      <c r="I73" t="s">
+        <v>72</v>
+      </c>
+      <c r="J73" t="s">
+        <v>103</v>
+      </c>
+      <c r="K73" s="2">
+        <v>43038</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F74" t="s">
+        <v>83</v>
+      </c>
+      <c r="G74">
+        <v>26</v>
+      </c>
+      <c r="H74" t="s">
+        <v>4</v>
+      </c>
+      <c r="I74" t="s">
+        <v>72</v>
+      </c>
+      <c r="J74" t="s">
+        <v>103</v>
+      </c>
+      <c r="K74" s="2">
+        <v>43038</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F75" t="s">
+        <v>83</v>
+      </c>
+      <c r="G75">
+        <v>42</v>
+      </c>
+      <c r="H75" t="s">
+        <v>4</v>
+      </c>
+      <c r="I75" t="s">
+        <v>72</v>
+      </c>
+      <c r="J75" t="s">
+        <v>103</v>
+      </c>
+      <c r="K75" s="2">
+        <v>43038</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F76" t="s">
+        <v>83</v>
+      </c>
+      <c r="G76">
+        <v>47</v>
+      </c>
+      <c r="H76" t="s">
+        <v>4</v>
+      </c>
+      <c r="I76" t="s">
+        <v>72</v>
+      </c>
+      <c r="J76" t="s">
+        <v>103</v>
+      </c>
+      <c r="K76" s="2">
+        <v>43038</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F77" t="s">
+        <v>83</v>
+      </c>
+      <c r="G77">
         <v>66</v>
       </c>
-      <c r="H67" t="s">
-        <v>5</v>
-      </c>
-      <c r="I67" t="s">
-        <v>78</v>
-      </c>
-      <c r="K67" s="2">
+      <c r="H77" t="s">
+        <v>4</v>
+      </c>
+      <c r="I77" t="s">
+        <v>72</v>
+      </c>
+      <c r="J77" t="s">
+        <v>103</v>
+      </c>
+      <c r="K77" s="2">
+        <v>43038</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F78" t="s">
+        <v>83</v>
+      </c>
+      <c r="G78">
+        <v>66</v>
+      </c>
+      <c r="H78" t="s">
+        <v>4</v>
+      </c>
+      <c r="I78" t="s">
+        <v>72</v>
+      </c>
+      <c r="J78" t="s">
+        <v>115</v>
+      </c>
+      <c r="K78" s="2">
         <v>43038</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="\\carbon.research.sickkids.ca\rkafri\Rajesh\Justins_Code_for_Cell_Counts\PlateMap_09_29_2017_CycD1_CycE1.xlsx"/>
-    <hyperlink ref="A12" r:id="rId2"/>
-    <hyperlink ref="A13" r:id="rId3"/>
-    <hyperlink ref="A8" r:id="rId4"/>
-    <hyperlink ref="A31" r:id="rId5"/>
-    <hyperlink ref="A32" r:id="rId6"/>
-    <hyperlink ref="A35" r:id="rId7"/>
-    <hyperlink ref="A38" r:id="rId8"/>
-    <hyperlink ref="A39" r:id="rId9"/>
-    <hyperlink ref="A40" r:id="rId10"/>
-    <hyperlink ref="A45" r:id="rId11"/>
-    <hyperlink ref="A46" r:id="rId12"/>
-    <hyperlink ref="B26" r:id="rId13"/>
-    <hyperlink ref="B27:B46" r:id="rId14" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171024_D1_E1_P27.xlsx"/>
-    <hyperlink ref="A54" r:id="rId15"/>
-    <hyperlink ref="B47" r:id="rId16"/>
-    <hyperlink ref="A47" r:id="rId17"/>
-    <hyperlink ref="A61" r:id="rId18"/>
+    <hyperlink ref="A13" r:id="rId2"/>
+    <hyperlink ref="A14" r:id="rId3"/>
+    <hyperlink ref="A9" r:id="rId4"/>
+    <hyperlink ref="A36" r:id="rId5"/>
+    <hyperlink ref="A37" r:id="rId6"/>
+    <hyperlink ref="A41" r:id="rId7"/>
+    <hyperlink ref="A44" r:id="rId8"/>
+    <hyperlink ref="A45" r:id="rId9"/>
+    <hyperlink ref="A47" r:id="rId10"/>
+    <hyperlink ref="A52" r:id="rId11"/>
+    <hyperlink ref="A53" r:id="rId12"/>
+    <hyperlink ref="B31" r:id="rId13"/>
+    <hyperlink ref="A63" r:id="rId14"/>
+    <hyperlink ref="B55" r:id="rId15"/>
+    <hyperlink ref="A55" r:id="rId16"/>
+    <hyperlink ref="A71" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
   <tableParts count="1">
-    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId19"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>